<commit_message>
Base Code testing GITHub
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkw19\OneDrive\Documents\UiPath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AA946A-9BD6-4FA5-9769-9096605C4DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF69B4D9-2202-4657-92A6-447AD00CCB88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1815" windowWidth="26070" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -142,9 +142,6 @@
     <t>pwong@etihad.ae; pakwong@outlook.com</t>
   </si>
   <si>
-    <t>01-JUL-2020</t>
-  </si>
-  <si>
     <t>MessageType</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Name to show when sending emails</t>
   </si>
   <si>
-    <t>Air.dddd</t>
-  </si>
-  <si>
     <t>https://etihad.sharepoint.com/sites/CargoDeliveryWeeklyReporting/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=N2l95q&amp;cid=0abf213b%2D54e8%2D4d9e%2D89fb%2D8d7755b70d32&amp;FolderCTID=0x012000F4DAA0DC828C25489FE85163DCB5E324&amp;viewid=958e0609%2D4115%2D4d5c%2Db167%2Dd80b043f3b33&amp;id=%2Fsites%2FCargoDeliveryWeeklyReporting%2FShared%20Documents%2FGeneral%2FCargo%20Delivery%2FCargo%20IQ%20DAP%20Daily</t>
   </si>
   <si>
@@ -377,6 +371,36 @@
   </si>
   <si>
     <t>DAP Email To List</t>
+  </si>
+  <si>
+    <t>BIDAPReportURL</t>
+  </si>
+  <si>
+    <t>BIGHAReportURL</t>
+  </si>
+  <si>
+    <t>BIEvolutionReportURL</t>
+  </si>
+  <si>
+    <t>BI DAP Report URL</t>
+  </si>
+  <si>
+    <t>BI GHA Repor tURL</t>
+  </si>
+  <si>
+    <t>BI Evolution Report URL</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/groups/137777c9-2dfd-406e-b75d-c8c3f6183177/reports/37f57a93-c504-411c-bfac-d39c71ffe917/ReportSectionbacdba451a1017289020?noSignUpCheck=1</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/groups/137777c9-2dfd-406e-b75d-c8c3f6183177/reports/37f57a93-c504-411c-bfac-d39c71ffe917/ReportSection176e7ffa09d6b77bc221</t>
+  </si>
+  <si>
+    <t>16-SEP-2020</t>
+  </si>
+  <si>
+    <t>P@ss.168</t>
   </si>
 </sst>
 </file>
@@ -718,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,8 +836,8 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>48</v>
+      <c r="B8" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -865,13 +889,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,7 +903,7 @@
         <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
         <v>36</v>
@@ -890,7 +914,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
         <v>35</v>
@@ -898,230 +922,264 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
         <v>77</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B25" r:id="rId1" xr:uid="{A97A4CAF-BE58-46EC-91A0-C9CAF8BBF231}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{97054F06-510D-4C26-BD66-CAA218AD12CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1153,110 +1211,110 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>